<commit_message>
semana 28, 29, y 30
</commit_message>
<xml_diff>
--- a/semana/semana_completa_28.xlsx
+++ b/semana/semana_completa_28.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29130"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80F3D80A-0B26-4A5E-A08B-F10176CED2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3563E721-AC2B-463B-B138-B460AE9C1BC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="6" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -16,9 +16,6 @@
     <sheet name="Evidencia_vok" sheetId="6" r:id="rId6"/>
     <sheet name="Evidencia_ns" sheetId="7" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Detalle_VOK!$A$1:$F$1</definedName>
@@ -45,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2733" uniqueCount="546">
   <si>
     <t>c</t>
   </si>
@@ -1620,15 +1617,6 @@
   </si>
   <si>
     <t>cr</t>
-  </si>
-  <si>
-    <t>Norte</t>
-  </si>
-  <si>
-    <t>Poniente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poniente </t>
   </si>
   <si>
     <t>id_ruta</t>
@@ -2062,19 +2050,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="asignacion operaciones"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -32081,9 +32056,6 @@
       <c r="A2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>525</v>
-      </c>
       <c r="C2" s="11">
         <v>0.92268890325189357</v>
       </c>
@@ -32093,9 +32065,6 @@
       <c r="A3" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>525</v>
-      </c>
       <c r="C3" s="11">
         <v>0.9096002448729722</v>
       </c>
@@ -32105,9 +32074,6 @@
       <c r="A4" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>525</v>
-      </c>
       <c r="C4" s="11">
         <v>0.98605950212507587</v>
       </c>
@@ -32117,9 +32083,6 @@
       <c r="A5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>525</v>
-      </c>
       <c r="C5" s="11">
         <v>0.97388283759251504</v>
       </c>
@@ -32129,9 +32092,6 @@
       <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>526</v>
-      </c>
       <c r="C6" s="11">
         <v>0.86538461538461542</v>
       </c>
@@ -32141,9 +32101,6 @@
       <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>526</v>
-      </c>
       <c r="C7" s="11">
         <v>0.96370139267302934</v>
       </c>
@@ -32153,9 +32110,6 @@
       <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>525</v>
-      </c>
       <c r="C8" s="11">
         <v>0.91306576220738622</v>
       </c>
@@ -32165,9 +32119,6 @@
       <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>525</v>
-      </c>
       <c r="C9" s="11">
         <v>0.97612644822253625</v>
       </c>
@@ -32177,9 +32128,6 @@
       <c r="A10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>525</v>
-      </c>
       <c r="C10" s="11">
         <v>0.97135416666666663</v>
       </c>
@@ -32189,9 +32137,6 @@
       <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>526</v>
-      </c>
       <c r="C11" s="11">
         <v>0.9545644941478274</v>
       </c>
@@ -32201,9 +32146,6 @@
       <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
-        <v>525</v>
-      </c>
       <c r="C12" s="11">
         <v>1</v>
       </c>
@@ -32213,9 +32155,6 @@
       <c r="A13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
-        <v>526</v>
-      </c>
       <c r="C13" s="11">
         <v>0.98249999999999993</v>
       </c>
@@ -32225,9 +32164,6 @@
       <c r="A14" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="s">
-        <v>526</v>
-      </c>
       <c r="C14" s="11">
         <v>0.94405458089668615</v>
       </c>
@@ -32237,9 +32173,6 @@
       <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="s">
-        <v>526</v>
-      </c>
       <c r="C15" s="11">
         <v>0.96884645470580433</v>
       </c>
@@ -32249,9 +32182,6 @@
       <c r="A16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="s">
-        <v>526</v>
-      </c>
       <c r="C16" s="11">
         <v>0.91714205121335157</v>
       </c>
@@ -32261,9 +32191,6 @@
       <c r="A17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
-        <v>526</v>
-      </c>
       <c r="C17" s="11">
         <v>0.97460226653590509</v>
       </c>
@@ -32273,9 +32200,6 @@
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
-        <v>526</v>
-      </c>
       <c r="C18" s="11">
         <v>1</v>
       </c>
@@ -32285,9 +32209,6 @@
       <c r="A19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
-        <v>526</v>
-      </c>
       <c r="C19" s="11">
         <v>0.9385926559232185</v>
       </c>
@@ -32297,9 +32218,6 @@
       <c r="A20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="s">
-        <v>526</v>
-      </c>
       <c r="C20" s="11">
         <v>0.95219648025093606</v>
       </c>
@@ -32309,9 +32227,6 @@
       <c r="A21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B21" t="s">
-        <v>525</v>
-      </c>
       <c r="C21" s="11">
         <v>0.98333333333333328</v>
       </c>
@@ -32321,9 +32236,6 @@
       <c r="A22" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B22" t="s">
-        <v>526</v>
-      </c>
       <c r="C22" s="11">
         <v>0.85336168910810539</v>
       </c>
@@ -32333,9 +32245,6 @@
       <c r="A23" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B23" t="s">
-        <v>525</v>
-      </c>
       <c r="C23" s="11">
         <v>1</v>
       </c>
@@ -32345,9 +32254,6 @@
       <c r="A24" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B24" t="s">
-        <v>525</v>
-      </c>
       <c r="C24" s="11">
         <v>0.68214285714285716</v>
       </c>
@@ -32357,9 +32263,6 @@
       <c r="A25" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B25" t="s">
-        <v>525</v>
-      </c>
       <c r="C25" s="11">
         <v>0.82106331884605699</v>
       </c>
@@ -32369,9 +32272,6 @@
       <c r="A26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B26" t="s">
-        <v>525</v>
-      </c>
       <c r="C26" s="11">
         <v>0.96448089966026163</v>
       </c>
@@ -32381,9 +32281,6 @@
       <c r="A27" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B27" t="s">
-        <v>525</v>
-      </c>
       <c r="C27" s="11">
         <v>0.84226190476190477</v>
       </c>
@@ -32393,9 +32290,6 @@
       <c r="A28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B28" t="s">
-        <v>525</v>
-      </c>
       <c r="C28" s="11">
         <v>0.99217715408603535</v>
       </c>
@@ -32405,9 +32299,6 @@
       <c r="A29" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B29" t="s">
-        <v>526</v>
-      </c>
       <c r="C29" s="11">
         <v>0.98252260080820453</v>
       </c>
@@ -32417,9 +32308,6 @@
       <c r="A30" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B30" t="s">
-        <v>526</v>
-      </c>
       <c r="C30" s="11">
         <v>1</v>
       </c>
@@ -32429,9 +32317,6 @@
       <c r="A31" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B31" t="s">
-        <v>526</v>
-      </c>
       <c r="C31" s="11">
         <v>0.71443808716535995</v>
       </c>
@@ -32441,9 +32326,6 @@
       <c r="A32" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B32" t="s">
-        <v>525</v>
-      </c>
       <c r="C32" s="11">
         <v>0.9</v>
       </c>
@@ -32453,9 +32335,6 @@
       <c r="A33" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B33" t="s">
-        <v>527</v>
-      </c>
       <c r="C33" s="11">
         <v>0.98852040816326525</v>
       </c>
@@ -32465,9 +32344,6 @@
       <c r="A34" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B34" t="s">
-        <v>526</v>
-      </c>
       <c r="C34" s="11">
         <v>0.97758458520991109</v>
       </c>
@@ -32477,9 +32353,6 @@
       <c r="A35" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B35" t="s">
-        <v>526</v>
-      </c>
       <c r="C35" s="11">
         <v>0.92361172915944889</v>
       </c>
@@ -32489,9 +32362,6 @@
       <c r="A36" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B36" t="s">
-        <v>526</v>
-      </c>
       <c r="C36" s="11">
         <v>0.93541666666666667</v>
       </c>
@@ -32501,9 +32371,6 @@
       <c r="A37" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B37" t="s">
-        <v>526</v>
-      </c>
       <c r="C37" s="11">
         <v>0.5</v>
       </c>
@@ -32513,9 +32380,6 @@
       <c r="A38" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B38" t="s">
-        <v>526</v>
-      </c>
       <c r="C38" s="11">
         <v>0.90691210257020882</v>
       </c>
@@ -32525,9 +32389,6 @@
       <c r="A39" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B39" t="s">
-        <v>526</v>
-      </c>
       <c r="C39" s="11">
         <v>0.99247493734335801</v>
       </c>
@@ -32537,9 +32398,6 @@
       <c r="A40" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B40" t="s">
-        <v>525</v>
-      </c>
       <c r="C40" s="11">
         <v>0.95454545454545459</v>
       </c>
@@ -32548,9 +32406,6 @@
     <row r="41" spans="1:5">
       <c r="A41" s="20" t="s">
         <v>48</v>
-      </c>
-      <c r="B41" t="s">
-        <v>526</v>
       </c>
       <c r="C41" s="11">
         <v>0.89593225402048948</v>
@@ -32674,16 +32529,16 @@
         <v>522</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>531</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>524</v>
@@ -32723,22 +32578,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="14" t="s">
+        <v>529</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>530</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>533</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>534</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>535</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>536</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -33048,86 +32903,86 @@
     </row>
     <row r="86" spans="4:6">
       <c r="D86" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="E86" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F86" s="43" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="87" spans="4:6">
       <c r="D87" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E87" t="s">
+        <v>536</v>
+      </c>
+      <c r="F87" s="43" t="s">
         <v>539</v>
-      </c>
-      <c r="F87" s="43" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="88" spans="4:6" ht="30.75">
       <c r="D88" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E88" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F88" s="43" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="89" spans="4:6">
       <c r="D89" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E89" t="s">
+        <v>540</v>
+      </c>
+      <c r="F89" s="43" t="s">
         <v>543</v>
-      </c>
-      <c r="F89" s="43" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="90" spans="4:6">
       <c r="D90" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E90" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F90" s="43"/>
     </row>
     <row r="91" spans="4:6">
       <c r="D91" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="E91" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F91" s="43"/>
     </row>
     <row r="92" spans="4:6">
       <c r="D92" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E92" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F92" s="43" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="93" spans="4:6">
       <c r="D93" t="s">
+        <v>542</v>
+      </c>
+      <c r="E93" t="s">
+        <v>536</v>
+      </c>
+      <c r="F93" s="43" t="s">
         <v>545</v>
-      </c>
-      <c r="E93" t="s">
-        <v>539</v>
-      </c>
-      <c r="F93" s="43" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="94" spans="4:6">

</xml_diff>